<commit_message>
Made all hashes lowercase and filled in some hashes.
</commit_message>
<xml_diff>
--- a/Docs/Missing Games (24 September 2025).xlsx
+++ b/Docs/Missing Games (24 September 2025).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unofficial-RA-DATs\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83B8316-51AF-4177-8583-9A563D375936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E428DBD2-54AE-4E97-A6FF-E8A3D1B85D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Sega Genesis" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <sheet name="21 - Sony PlayStation 2" sheetId="8" r:id="rId9"/>
     <sheet name="27 - Arcade" sheetId="9" r:id="rId10"/>
     <sheet name="33 - Sega SG-1000" sheetId="10" r:id="rId11"/>
-    <sheet name="41 - Sony Playstation Portable" sheetId="11" r:id="rId12"/>
+    <sheet name="38 - Apple II" sheetId="13" r:id="rId12"/>
+    <sheet name="41 - Sony Playstation Portable" sheetId="11" r:id="rId13"/>
+    <sheet name="47 - NEC PC8801" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="604">
   <si>
     <t>GAME NAME</t>
   </si>
@@ -1770,6 +1772,84 @@
   </si>
   <si>
     <t>Only Disc 1 of this Edition is linked. Will wait for the other discs to be linked 1st.</t>
+  </si>
+  <si>
+    <t>King's Quest - disk A.dsk[appleasimov][theblade]</t>
+  </si>
+  <si>
+    <t>34f8869a6f033195023d3b60ce814ecd</t>
+  </si>
+  <si>
+    <t>Duplicate rom with different hash.</t>
+  </si>
+  <si>
+    <t>Space Quest 1 - Disk 1 - Front.dsk[appleasimov][theblade]</t>
+  </si>
+  <si>
+    <t>68b4687a664173975d280789b55ed51a</t>
+  </si>
+  <si>
+    <t>Wheel of Fortune (1987)(Sharedata)(US).dsk</t>
+  </si>
+  <si>
+    <t>94a70fed0893d60084b59d4e4a955924</t>
+  </si>
+  <si>
+    <t>This is a single disk rom while the roms in the dat are multi-disk. Might swop them around in the future.</t>
+  </si>
+  <si>
+    <t>Wasteland (1987)(Electronic Arts)(Disk 1 of 4 Side B)[cr Crackforce][a].dsk</t>
+  </si>
+  <si>
+    <t>9fc328d5eab51b6b52952f941160adf7</t>
+  </si>
+  <si>
+    <t>This as an alternate disk and isn't needed at the moment.</t>
+  </si>
+  <si>
+    <t>Paranoiak (1984) (Froggy Software) (Chip Select Crack) (Disk 2)</t>
+  </si>
+  <si>
+    <t>fc40e6016f06eb748ead9b072c53b6aa</t>
+  </si>
+  <si>
+    <t>This is a Disk 2 rom with no Disk 1 linked while the roms in the dat are multi-disk.</t>
+  </si>
+  <si>
+    <t>The Scheme (music mode) (Disk 1).d88</t>
+  </si>
+  <si>
+    <t>8dab8eb445c9b7d4dd143b1df75017a6</t>
+  </si>
+  <si>
+    <t>The Scheme [Set 2] (Disk 1).d88</t>
+  </si>
+  <si>
+    <t>b170f9e16671c8c3e14345b75d80b9a5</t>
+  </si>
+  <si>
+    <t>This is only a Set 2 disk with no disk 2 linked and isn't needed at the moment.</t>
+  </si>
+  <si>
+    <t>This is only a music mode disk with no disk 2 linked and isn't needed at the moment.</t>
+  </si>
+  <si>
+    <t>Ys (Disk A).d88</t>
+  </si>
+  <si>
+    <t>b838e8767516ffaa5b469bb9e319f5a5</t>
+  </si>
+  <si>
+    <t>This is a Disk A rom with no Disk B linked.</t>
+  </si>
+  <si>
+    <t>Battle Skin Panic (Disk A) [Alt 1].d88</t>
+  </si>
+  <si>
+    <t>b89932234465e1bb1aa710bc8759b615</t>
+  </si>
+  <si>
+    <t>This is an alternate Disk A rom and isn't needed at the moment.</t>
   </si>
 </sst>
 </file>
@@ -1827,13 +1907,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1855,6 +1928,11 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1864,7 +1942,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1898,6 +1976,21 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1950,25 +2043,25 @@
     </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2233,18 +2326,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63" style="23" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="24" customWidth="1"/>
-    <col min="3" max="3" width="94.42578125" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="63" style="22" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="94.42578125" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2255,19 +2348,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>544</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>545</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="32"/>
+      <c r="C3" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2281,18 +2374,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="33" style="24" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="51.5703125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="33" style="23" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>484</v>
       </c>
@@ -2304,10 +2397,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>547</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>548</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -2321,12 +2414,99 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED3C4D5-8105-4AFE-8DDD-C1834B6448C4}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>581</v>
+      </c>
+      <c r="B3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B4" t="s">
+        <v>584</v>
+      </c>
+      <c r="C4" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>586</v>
+      </c>
+      <c r="B5" t="s">
+        <v>587</v>
+      </c>
+      <c r="C5" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B6" t="s">
+        <v>590</v>
+      </c>
+      <c r="C6" t="s">
+        <v>591</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C369"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2517,7 @@
     <col min="4" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2348,7 +2528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>549</v>
       </c>
@@ -2370,7 +2550,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="27" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>554</v>
       </c>
@@ -2381,7 +2561,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="27" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>557</v>
       </c>
@@ -4245,6 +4425,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57818AC2-4463-4A09-8140-251C396204BF}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="27" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3" t="s">
+        <v>595</v>
+      </c>
+      <c r="C3" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>601</v>
+      </c>
+      <c r="B5" t="s">
+        <v>602</v>
+      </c>
+      <c r="C5" t="s">
+        <v>603</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4252,15 +4509,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C183"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="103.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" style="11" customWidth="1"/>
     <col min="3" max="3" width="60.5703125" style="12" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="11"/>
@@ -6268,11 +6525,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="20" t="s">
+    <row r="183" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A183" s="32" t="s">
         <v>374</v>
       </c>
-      <c r="B183" s="20" t="s">
+      <c r="B183" s="32" t="s">
         <v>375</v>
       </c>
       <c r="C183" s="17" t="s">
@@ -6296,7 +6553,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="103.140625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="103.140625" style="20" customWidth="1"/>
     <col min="2" max="2" width="57.42578125" customWidth="1"/>
     <col min="3" max="3" width="100.140625" customWidth="1"/>
   </cols>
@@ -6334,7 +6591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>380</v>
       </c>
@@ -6356,19 +6613,19 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="64.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6952,18 +7209,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.5703125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="75.5703125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>484</v>
       </c>
@@ -7006,7 +7263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EA685A-6B74-42D3-8C63-E13E4551FD07}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -7017,7 +7274,7 @@
     <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>484</v>
       </c>
@@ -7054,13 +7311,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="49.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>484</v>
       </c>
@@ -7072,10 +7329,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>490</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>491</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -7099,13 +7356,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" style="23" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="43.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="70.140625" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>484</v>
       </c>
@@ -7117,10 +7374,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>492</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>493</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -7139,17 +7396,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="112.5703125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="112.5703125" style="20" customWidth="1"/>
     <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="3" width="98.85546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="98.85546875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="27" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -7194,7 +7451,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>500</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -7205,7 +7462,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>500</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -7447,7 +7704,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="20" t="s">
         <v>569</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -7458,7 +7715,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="20" t="s">
         <v>571</v>
       </c>
       <c r="B29" s="19" t="s">

</xml_diff>